<commit_message>
fix: make most classes inherit from NamedEntity to be addressable.
</commit_message>
<xml_diff>
--- a/project/excel/smoc_schema.xlsx
+++ b/project/excel/smoc_schema.xlsx
@@ -459,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,21 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>has_reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -582,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,6 +619,21 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>omics_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -623,7 +653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -642,6 +672,21 @@
           <t>collector</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -654,7 +699,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -681,6 +726,21 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>has_reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -700,115 +760,150 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>taxon_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>source_uri</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>has_sequence</t>
+          <t>sequence_md5</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>taxon_id</t>
+          <t>source_uri</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>source_uri</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>data_format</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>sequence_md5</t>
+          <t>has_sample</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>source_uri</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>data_format</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_sample</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>has_reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -828,7 +923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +950,21 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>has_reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>

</xml_diff>